<commit_message>
Exported all of the Map Overlays
</commit_message>
<xml_diff>
--- a/Lidar/QGIS/Heightmap/GleneagleGC_MaxMin.xlsx
+++ b/Lidar/QGIS/Heightmap/GleneagleGC_MaxMin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OPCDProjects\GleneagleGC\Lidar\QGIS\Heightmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6C0078-3441-4868-8B5C-CE7C9639267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB19BDE-1EE9-4DD7-A36E-A3DFB8011074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -936,7 +936,9 @@
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <v>710.12</v>
+      </c>
       <c r="D5" s="30" t="s">
         <v>12</v>
       </c>
@@ -952,7 +954,9 @@
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5">
+        <v>603.05799999999999</v>
+      </c>
       <c r="D6" s="30"/>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
@@ -968,7 +972,7 @@
       </c>
       <c r="C7" s="13">
         <f>(C5-C6)*0.3048</f>
-        <v>0</v>
+        <v>32.632497600000008</v>
       </c>
       <c r="D7" s="11"/>
     </row>
@@ -1012,7 +1016,9 @@
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5">
+        <v>726.69</v>
+      </c>
       <c r="D11" s="30" t="s">
         <v>13</v>
       </c>
@@ -1028,7 +1034,9 @@
       <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5">
+        <v>599.52700000000004</v>
+      </c>
       <c r="D12" s="30"/>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
@@ -1044,7 +1052,7 @@
       </c>
       <c r="C13" s="13">
         <f>(C11-C12)*0.3048</f>
-        <v>0</v>
+        <v>38.759282400000004</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="24"/>
@@ -1092,7 +1100,7 @@
       </c>
       <c r="D19" s="10">
         <f>(C12*0.3048)-(C6*0.3048)</f>
-        <v>0</v>
+        <v>-1.0762488000000019</v>
       </c>
       <c r="E19" s="18">
         <f>(C4-C10)/2</f>

</xml_diff>